<commit_message>
Execute total_phases.xlsx once more
</commit_message>
<xml_diff>
--- a/data/interim/interaction_matrices/willem_2012/phases/total_phases.xlsx
+++ b/data/interim/interaction_matrices/willem_2012/phases/total_phases.xlsx
@@ -439,802 +439,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>8.61114955807408</v>
-      </c>
-      <c r="C2">
-        <v>0.833935019404327</v>
-      </c>
-      <c r="D2">
-        <v>0.5682801153101441</v>
-      </c>
-      <c r="E2">
-        <v>1.75586950288063</v>
-      </c>
-      <c r="F2">
-        <v>2.11664332286198</v>
-      </c>
-      <c r="G2">
-        <v>1.07760315247374</v>
-      </c>
-      <c r="H2">
-        <v>0.930447609887303</v>
-      </c>
-      <c r="I2">
-        <v>0.388143895268713</v>
-      </c>
-      <c r="J2">
-        <v>0.194554932281382</v>
-      </c>
-      <c r="K2">
-        <v>0.0208399703766592</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>1.62464948703735</v>
-      </c>
-      <c r="C3">
-        <v>10.2024509978958</v>
-      </c>
-      <c r="D3">
-        <v>2.3531644554918</v>
-      </c>
-      <c r="E3">
-        <v>3.11148900845971</v>
-      </c>
-      <c r="F3">
-        <v>2.1581076325096</v>
-      </c>
-      <c r="G3">
-        <v>1.83025706646436</v>
-      </c>
-      <c r="H3">
-        <v>0.381448289384702</v>
-      </c>
-      <c r="I3">
-        <v>0.349867966315856</v>
-      </c>
-      <c r="J3">
-        <v>0.111544111686216</v>
-      </c>
-      <c r="K3">
-        <v>0.0918308668798731</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>0.9048016366270841</v>
-      </c>
-      <c r="C4">
-        <v>1.92316138872708</v>
-      </c>
-      <c r="D4">
-        <v>6.15189471041101</v>
-      </c>
-      <c r="E4">
-        <v>3.12873167064806</v>
-      </c>
-      <c r="F4">
-        <v>2.2125539396801</v>
-      </c>
-      <c r="G4">
-        <v>3.27484972895714</v>
-      </c>
-      <c r="H4">
-        <v>0.8422105776160601</v>
-      </c>
-      <c r="I4">
-        <v>0.336796325334897</v>
-      </c>
-      <c r="J4">
-        <v>0.154446742604574</v>
-      </c>
-      <c r="K4">
-        <v>0.10279999442724</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>1.83312729034624</v>
-      </c>
-      <c r="C5">
-        <v>1.66740535554375</v>
-      </c>
-      <c r="D5">
-        <v>2.05152960228826</v>
-      </c>
-      <c r="E5">
-        <v>5.27218354538779</v>
-      </c>
-      <c r="F5">
-        <v>4.170866949193</v>
-      </c>
-      <c r="G5">
-        <v>4.43751605593746</v>
-      </c>
-      <c r="H5">
-        <v>2.23509140024301</v>
-      </c>
-      <c r="I5">
-        <v>0.5238988562048279</v>
-      </c>
-      <c r="J5">
-        <v>0.310510153563409</v>
-      </c>
-      <c r="K5">
-        <v>0.203968808302052</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>2.05061850063921</v>
-      </c>
-      <c r="C6">
-        <v>1.07320533968284</v>
-      </c>
-      <c r="D6">
-        <v>1.34629471183976</v>
-      </c>
-      <c r="E6">
-        <v>3.87046495272467</v>
-      </c>
-      <c r="F6">
-        <v>5.38623365438201</v>
-      </c>
-      <c r="G6">
-        <v>4.03246549227232</v>
-      </c>
-      <c r="H6">
-        <v>2.1837257370587</v>
-      </c>
-      <c r="I6">
-        <v>0.9693050987879929</v>
-      </c>
-      <c r="J6">
-        <v>0.454288546176596</v>
-      </c>
-      <c r="K6">
-        <v>0.164078026856949</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>1.00280448519873</v>
-      </c>
-      <c r="C7">
-        <v>0.8742628827204059</v>
-      </c>
-      <c r="D7">
-        <v>1.91407025160079</v>
-      </c>
-      <c r="E7">
-        <v>3.95545970650394</v>
-      </c>
-      <c r="F7">
-        <v>3.8733869389069</v>
-      </c>
-      <c r="G7">
-        <v>5.2402877879435</v>
-      </c>
-      <c r="H7">
-        <v>2.52785646912505</v>
-      </c>
-      <c r="I7">
-        <v>1.22236571064588</v>
-      </c>
-      <c r="J7">
-        <v>0.763777653609236</v>
-      </c>
-      <c r="K7">
-        <v>0.145128421051211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>1.02952012568295</v>
-      </c>
-      <c r="C8">
-        <v>0.216646222851063</v>
-      </c>
-      <c r="D8">
-        <v>0.5852921377741911</v>
-      </c>
-      <c r="E8">
-        <v>2.36885139316917</v>
-      </c>
-      <c r="F8">
-        <v>2.49404232042816</v>
-      </c>
-      <c r="G8">
-        <v>3.00564658263296</v>
-      </c>
-      <c r="H8">
-        <v>2.58577059395861</v>
-      </c>
-      <c r="I8">
-        <v>0.81215397604949</v>
-      </c>
-      <c r="J8">
-        <v>0.461924748042262</v>
-      </c>
-      <c r="K8">
-        <v>0.191576374694039</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>0.619371762519808</v>
-      </c>
-      <c r="C9">
-        <v>0.286573056751293</v>
-      </c>
-      <c r="D9">
-        <v>0.337547634348598</v>
-      </c>
-      <c r="E9">
-        <v>0.8007661473487521</v>
-      </c>
-      <c r="F9">
-        <v>1.59654788459805</v>
-      </c>
-      <c r="G9">
-        <v>2.09605360887651</v>
-      </c>
-      <c r="H9">
-        <v>1.17126212654357</v>
-      </c>
-      <c r="I9">
-        <v>1.99325316005328</v>
-      </c>
-      <c r="J9">
-        <v>0.8470941302027479</v>
-      </c>
-      <c r="K9">
-        <v>0.123857848011403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>0.39848572365866</v>
-      </c>
-      <c r="C10">
-        <v>0.117270750465588</v>
-      </c>
-      <c r="D10">
-        <v>0.198681924011471</v>
-      </c>
-      <c r="E10">
-        <v>0.609180426001695</v>
-      </c>
-      <c r="F10">
-        <v>0.9604286755057589</v>
-      </c>
-      <c r="G10">
-        <v>1.68104776918448</v>
-      </c>
-      <c r="H10">
-        <v>0.855064420629336</v>
-      </c>
-      <c r="I10">
-        <v>1.08728538902178</v>
-      </c>
-      <c r="J10">
-        <v>0.913586801881675</v>
-      </c>
-      <c r="K10">
-        <v>0.302370126956865</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>0.125360588349138</v>
-      </c>
-      <c r="C11">
-        <v>0.283547055857157</v>
-      </c>
-      <c r="D11">
-        <v>0.388388263729695</v>
-      </c>
-      <c r="E11">
-        <v>1.17524197889506</v>
-      </c>
-      <c r="F11">
-        <v>1.01877237186244</v>
-      </c>
-      <c r="G11">
-        <v>0.9381212643774459</v>
-      </c>
-      <c r="H11">
-        <v>1.04150883593759</v>
-      </c>
-      <c r="I11">
-        <v>0.466905309532618</v>
-      </c>
-      <c r="J11">
-        <v>0.888039503366962</v>
-      </c>
-      <c r="K11">
-        <v>1.12414684090862</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>4.95011276316063</v>
-      </c>
-      <c r="C2">
-        <v>0.428506302982155</v>
-      </c>
-      <c r="D2">
-        <v>0.4012594048414529</v>
-      </c>
-      <c r="E2">
-        <v>1.12482184011456</v>
-      </c>
-      <c r="F2">
-        <v>1.42839432233008</v>
-      </c>
-      <c r="G2">
-        <v>0.6389189759977479</v>
-      </c>
-      <c r="H2">
-        <v>0.5970939246885589</v>
-      </c>
-      <c r="I2">
-        <v>0.322965160690765</v>
-      </c>
-      <c r="J2">
-        <v>0.174468874310895</v>
-      </c>
-      <c r="K2">
-        <v>0.0143797737499922</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>0.834804306250982</v>
-      </c>
-      <c r="C3">
-        <v>5.34714348739267</v>
-      </c>
-      <c r="D3">
-        <v>1.06745117850894</v>
-      </c>
-      <c r="E3">
-        <v>1.25202084885098</v>
-      </c>
-      <c r="F3">
-        <v>1.1723976544487</v>
-      </c>
-      <c r="G3">
-        <v>0.877439672446519</v>
-      </c>
-      <c r="H3">
-        <v>0.152597245857336</v>
-      </c>
-      <c r="I3">
-        <v>0.251382149255555</v>
-      </c>
-      <c r="J3">
-        <v>0.0706499964120099</v>
-      </c>
-      <c r="K3">
-        <v>0.0742989834268732</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>0.6388753652138829</v>
-      </c>
-      <c r="C4">
-        <v>0.8723915942502929</v>
-      </c>
-      <c r="D4">
-        <v>2.58301722544248</v>
-      </c>
-      <c r="E4">
-        <v>1.19835843870504</v>
-      </c>
-      <c r="F4">
-        <v>0.8079111357607449</v>
-      </c>
-      <c r="G4">
-        <v>1.43862569246641</v>
-      </c>
-      <c r="H4">
-        <v>0.351962774777115</v>
-      </c>
-      <c r="I4">
-        <v>0.117325315772357</v>
-      </c>
-      <c r="J4">
-        <v>0.0738300834471524</v>
-      </c>
-      <c r="K4">
-        <v>0.0592802238261513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>1.1743136995709</v>
-      </c>
-      <c r="C5">
-        <v>0.670941231979473</v>
-      </c>
-      <c r="D5">
-        <v>0.785771382768054</v>
-      </c>
-      <c r="E5">
-        <v>2.45158747703602</v>
-      </c>
-      <c r="F5">
-        <v>1.44196131998854</v>
-      </c>
-      <c r="G5">
-        <v>1.620038093953</v>
-      </c>
-      <c r="H5">
-        <v>0.9017294789904959</v>
-      </c>
-      <c r="I5">
-        <v>0.210875254102876</v>
-      </c>
-      <c r="J5">
-        <v>0.149284442880086</v>
-      </c>
-      <c r="K5">
-        <v>0.08761361238041099</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>1.38383817053199</v>
-      </c>
-      <c r="C6">
-        <v>0.583021626925453</v>
-      </c>
-      <c r="D6">
-        <v>0.49159772794891</v>
-      </c>
-      <c r="E6">
-        <v>1.33810567927133</v>
-      </c>
-      <c r="F6">
-        <v>2.39231092782578</v>
-      </c>
-      <c r="G6">
-        <v>1.523002666951</v>
-      </c>
-      <c r="H6">
-        <v>0.726209612092817</v>
-      </c>
-      <c r="I6">
-        <v>0.430966501354483</v>
-      </c>
-      <c r="J6">
-        <v>0.205411253946177</v>
-      </c>
-      <c r="K6">
-        <v>0.103627618358709</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>0.5945702862304271</v>
-      </c>
-      <c r="C7">
-        <v>0.419128521070666</v>
-      </c>
-      <c r="D7">
-        <v>0.840841830631239</v>
-      </c>
-      <c r="E7">
-        <v>1.44405007730812</v>
-      </c>
-      <c r="F7">
-        <v>1.46292104653924</v>
-      </c>
-      <c r="G7">
-        <v>2.37606867486476</v>
-      </c>
-      <c r="H7">
-        <v>1.09707753987727</v>
-      </c>
-      <c r="I7">
-        <v>0.50294989247226</v>
-      </c>
-      <c r="J7">
-        <v>0.390832111159366</v>
-      </c>
-      <c r="K7">
-        <v>0.0892548138875776</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>0.66067149386772</v>
-      </c>
-      <c r="C8">
-        <v>0.0866686726680405</v>
-      </c>
-      <c r="D8">
-        <v>0.244595651421685</v>
-      </c>
-      <c r="E8">
-        <v>0.9556938621553009</v>
-      </c>
-      <c r="F8">
-        <v>0.8294070428920859</v>
-      </c>
-      <c r="G8">
-        <v>1.30443614931856</v>
-      </c>
-      <c r="H8">
-        <v>1.40751691798508</v>
-      </c>
-      <c r="I8">
-        <v>0.349826944611701</v>
-      </c>
-      <c r="J8">
-        <v>0.249570552933473</v>
-      </c>
-      <c r="K8">
-        <v>0.107629463462997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>0.515364284348841</v>
-      </c>
-      <c r="C9">
-        <v>0.205904392115276</v>
-      </c>
-      <c r="D9">
-        <v>0.117587039433349</v>
-      </c>
-      <c r="E9">
-        <v>0.3223174908653161</v>
-      </c>
-      <c r="F9">
-        <v>0.709847350365188</v>
-      </c>
-      <c r="G9">
-        <v>0.8624341537227019</v>
-      </c>
-      <c r="H9">
-        <v>0.5045090748200329</v>
-      </c>
-      <c r="I9">
-        <v>1.1961521443084</v>
-      </c>
-      <c r="J9">
-        <v>0.531364697589447</v>
-      </c>
-      <c r="K9">
-        <v>0.0733814531738432</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10">
-        <v>0.357345634060503</v>
-      </c>
-      <c r="C10">
-        <v>0.0742771444801538</v>
-      </c>
-      <c r="D10">
-        <v>0.0949758006017882</v>
-      </c>
-      <c r="E10">
-        <v>0.2928766079481699</v>
-      </c>
-      <c r="F10">
-        <v>0.434267736270008</v>
-      </c>
-      <c r="G10">
-        <v>0.860207739104985</v>
-      </c>
-      <c r="H10">
-        <v>0.46197762980796</v>
-      </c>
-      <c r="I10">
-        <v>0.682031726264824</v>
-      </c>
-      <c r="J10">
-        <v>0.501777727933594</v>
-      </c>
-      <c r="K10">
-        <v>0.112484256265844</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11">
-        <v>0.08649997409043771</v>
-      </c>
-      <c r="C11">
-        <v>0.229413689750183</v>
-      </c>
-      <c r="D11">
-        <v>0.223966385734023</v>
-      </c>
-      <c r="E11">
-        <v>0.504818339868996</v>
-      </c>
-      <c r="F11">
-        <v>0.643431400097229</v>
-      </c>
-      <c r="G11">
-        <v>0.576949974715438</v>
-      </c>
-      <c r="H11">
-        <v>0.5851297550804979</v>
-      </c>
-      <c r="I11">
-        <v>0.2766251041672571</v>
-      </c>
-      <c r="J11">
-        <v>0.330358240333616</v>
-      </c>
-      <c r="K11">
-        <v>0.246486184482509</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K11"/>

</xml_diff>